<commit_message>
finished descriptives and corrs
</commit_message>
<xml_diff>
--- a/Output/CorrelationsMain.xlsx
+++ b/Output/CorrelationsMain.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,50 +365,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>persuasion_self</t>
+          <t>persuasion</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>persuasion_partner</t>
+          <t>pressure</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>pressure_self</t>
+          <t>pushing</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>pressure_partner</t>
+          <t>pa_sub</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>pushing_self</t>
+          <t>pa_obj</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>pushing_partner</t>
+          <t>aff</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>pa_sub</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>pa_obj</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>aff</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>reactance</t>
         </is>
@@ -417,7 +402,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>persuasion_self</t>
+          <t>persuasion</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -427,45 +412,30 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.46***</t>
+          <t>0.21***</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.21***</t>
+          <t>0.40***</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.10***</t>
+          <t>0.17***</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.40***</t>
+          <t>0.07***</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.26***</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>0.17***</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0.07***</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
         <is>
           <t>-0.05</t>
         </is>
@@ -474,511 +444,250 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>persuasion_partner</t>
+          <t>pressure</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.00***</t>
+          <t>0.30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[0.20]</t>
+          <t>[0.55]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.10***</t>
+          <t>0.28***</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.21***</t>
+          <t>-0.03</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>-0.04*</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-0.01</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>0.26***</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0.40***</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0.18***</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.06***</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0.02</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>pressure_self</t>
+          <t>pushing</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.30</t>
+          <t>0.63***</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.30</t>
+          <t>0.40*</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[0.55]</t>
+          <t>[0.08]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.75***</t>
+          <t>0.14***</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.28***</t>
+          <t>0.05**</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.17***</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>-0.03</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>-0.04*</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>-0.01</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0.26***</t>
+          <t>0.07*</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>pressure_partner</t>
+          <t>pa_sub</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.30</t>
+          <t>0.27</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.30</t>
+          <t>-0.10</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.00***</t>
+          <t>0.24</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[0.55]</t>
+          <t>[0.15]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.17***</t>
+          <t>0.31***</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.28***</t>
+          <t>0.20***</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>-0.00</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>-0.03</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>0.02</t>
+          <t>-0.04</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>pushing_self</t>
+          <t>pa_obj</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.63***</t>
+          <t>0.13</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.63***</t>
+          <t>-0.08</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.40*</t>
+          <t>0.27</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.40*</t>
+          <t>0.51***</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[0.08]</t>
+          <t>[0.13]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.62***</t>
+          <t>0.19***</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.14***</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0.05**</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>0.07*</t>
+          <t>0.06</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>pushing_partner</t>
+          <t>aff</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.63***</t>
+          <t>0.28</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.63***</t>
+          <t>-0.07</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.40*</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.40*</t>
+          <t>0.52***</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1.00***</t>
+          <t>0.22</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[0.08]</t>
+          <t>[0.28]</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.15***</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>0.06***</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>0.04**</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>-0.07*</t>
+          <t>-0.01</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>pa_sub</t>
+          <t>reactance</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.27</t>
+          <t>0.18</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.27</t>
+          <t>0.23</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-0.10</t>
+          <t>0.11</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-0.10</t>
+          <t>0.06</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.38*</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>-0.12</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
-        <is>
-          <t>[0.15]</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0.31***</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>0.20***</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>-0.04</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>pa_obj</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0.13</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0.13</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>-0.08</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>-0.08</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0.27</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>0.27</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>0.51***</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>[0.13]</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>0.19***</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>aff</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>-0.07</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>-0.07</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>0.52***</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>0.22</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>[0.28]</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>-0.01</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>reactance</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>0.18</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>0.18</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0.23</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0.23</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0.11</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0.11</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0.38*</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>-0.12</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
         <is>
           <t>[0.42]</t>
         </is>

</xml_diff>